<commit_message>
add updated 2022-2023 data and OTP status
</commit_message>
<xml_diff>
--- a/Data/StateYear_Income_Unemployed/State_Population_Unemployment_Income.xlsx
+++ b/Data/StateYear_Income_Unemployed/State_Population_Unemployment_Income.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baileywellen/Library/CloudStorage/Box-Box/02.Classes/Year1/2024 Spring/Health Economics/FinalPaper/sud_treatment_profitstatus/Data/StateYear_Income_Unemployed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E06557F-5D03-C84C-A6DB-E05813C0218B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66985E5E-0FBE-7645-B05B-8B11A41C0209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -1638,7 +1638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3832"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1217" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -22193,11 +22195,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D958E503-9413-704D-9FA5-F3783D2AEB80}">
   <dimension ref="A1:I154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I154"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="60.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">

</xml_diff>